<commit_message>
Final changes to file split logic
</commit_message>
<xml_diff>
--- a/cloumns_across_years.xlsx
+++ b/cloumns_across_years.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aki/dev/Rick_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EC3D76-D682-9E44-979F-DE7E6880FA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA3F905-0F4F-5B46-9310-79B8D40E4474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="960" windowWidth="27200" windowHeight="16960" xr2:uid="{A063132B-9E1A-3C4D-9237-694C8A9C6683}"/>
+    <workbookView xWindow="39400" yWindow="2520" windowWidth="32900" windowHeight="19080" xr2:uid="{A063132B-9E1A-3C4D-9237-694C8A9C6683}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="195">
   <si>
     <t>HMDA cvf file columns over the years</t>
   </si>
@@ -570,13 +570,55 @@
     <t>77 application_date_indicator</t>
   </si>
   <si>
-    <t>'2019', '549300IQVXIW1VTW0D69', '45540', 'FL', '12119', '12119910300', 'C', 'Conventional:First Lien', 'Single Family (1-4 Units):Site-Built', 'Not Hispanic or Latino', 'White', 'Joint', '4', '0', '2', '1', '1', '1', '2', '2', '2', '255000.0', 'NA', 'NA', 'NA', '3', 'NA', 'NA', 'NA', 'NA', 'NA', '360', 'NA', 'NA', '2', '2', '2', '2', 'NA', '1', '1', '3', '5', '1', 'NA', '130', 'NA', '9', '9', '2', '', '', '', '', '2', '', '', '', '', '2', '2', '5', '', '', '', '', '5', '', '', '', '', '2', '2', '1', '2', '2', '2', '65-74', '65-74', 'Yes', 'Yes', '1', '3', '1', '', '', '', '', '10', '', '', '', '1633', '3.31000000000000005', '71300', '87', '460', '765', '36\n'</t>
-  </si>
-  <si>
     <t>'2017', '0000068601', 'National Credit Union Administration', 'NCUA', '5', 'Conventional', '1', 'One-to-four family dwelling (other than manufactured housing)', '1', 'Home purchase', '1', 'Owner-occupied as a principal dwelling', '1', '175', 'Preapproval was requested', '1', 'Loan originated', '1', '', '', 'Michigan', 'MI', '26', 'Alpena County', '7', '0002.00', 'Information not provided by applicant in mail', ' Internet', ' or telephone application', '3', 'Information not provided by applicant in mail', ' Internet', ' or telephone application', '3', 'Information not provided by applicant in mail', ' Internet', ' or telephone application', '6', '', '', '', '', '', '', '', '', 'Information not provided by applicant in mail', ' Internet', ' or telephone application', '6', '', '', '', '', '', '', '', '', 'Information not provided by applicant in mail', ' Internet', ' or telephone application', '3', 'Information not provided by applicant in mail', ' Internet', ' or telephone application', '3', '38', 'Loan was not originated or was not sold in calendar year covered by register', '0', '', '', '', '', '', '', '', 'Not a HOEPA loan', '2', 'Secured by a first lien', '1', '', '', '', '4272', '2.7899999618530273', '55800', '99.97000122070312', '1609', '2271', '\n'</t>
   </si>
   <si>
     <t>Sample lines from 2017 and 2019</t>
+  </si>
+  <si>
+    <t>2019', '549300IQVXIW1VTW0D69', '45540', 'FL', '12119', '12119910300', 'C', 'Conventional:First Lien', 'Single Family (1-4 Units):Site-Built', 'Not Hispanic or Latino', 'White', 'Joint', '4', '0', '2', '1', '1', '1', '2', '2', '2', '255000.0', 'NA', 'NA', 'NA', '3', 'NA', 'NA', 'NA', 'NA', 'NA', '360', 'NA', 'NA', '2', '2', '2', '2', 'NA', '1', '1', '3', '5', '1', 'NA', '130', 'NA', '9', '9', '2', '', '', '', '', '2', '', '', '', '', '2', '2', '5', '', '', '', '', '5', '', '', '', '', '2', '2', '1', '2', '2', '2', '65-74', '65-74', 'Yes', 'Yes', '1', '3', '1', '', '', '', '', '10', '', '', '', '1633', '3.31000000000000005', '71300', '87', '460', '765', '36\n'</t>
+  </si>
+  <si>
+    <t>Year maps</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Our DB field names</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>lender_id</t>
+  </si>
+  <si>
+    <t>agency_code</t>
+  </si>
+  <si>
+    <t>loan_type</t>
+  </si>
+  <si>
+    <t>property_type</t>
+  </si>
+  <si>
+    <t>loan_amount_in_000s</t>
+  </si>
+  <si>
+    <t>DB joins</t>
+  </si>
+  <si>
+    <t>lei ON lender_id</t>
+  </si>
+  <si>
+    <t>2010-17</t>
+  </si>
+  <si>
+    <t>2018-19</t>
+  </si>
+  <si>
+    <t>respondent_id ON lender_id</t>
   </si>
 </sst>
 </file>
@@ -618,7 +660,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,6 +688,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -765,7 +813,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -789,6 +837,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1103,23 +1157,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46BE7AE-2223-7645-A256-2ED50F561D21}">
-  <dimension ref="A1:K108"/>
+  <dimension ref="A1:Q108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="9" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" customWidth="1"/>
+    <col min="14" max="14" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25" customWidth="1"/>
+    <col min="17" max="17" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q3" s="16"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>2010</v>
       </c>
@@ -1150,8 +1220,23 @@
       <c r="K4" s="3">
         <v>2019</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M4" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>100</v>
       </c>
@@ -1176,14 +1261,23 @@
       <c r="I5" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="14" t="s">
         <v>1</v>
       </c>
       <c r="K5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M5" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>101</v>
       </c>
@@ -1208,14 +1302,29 @@
       <c r="I6" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="14" t="s">
         <v>2</v>
       </c>
       <c r="K6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M6" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>102</v>
       </c>
@@ -1246,8 +1355,17 @@
       <c r="K7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>187</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>103</v>
       </c>
@@ -1278,8 +1396,17 @@
       <c r="K8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>188</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>104</v>
       </c>
@@ -1310,8 +1437,17 @@
       <c r="K9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M9" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>105</v>
       </c>
@@ -1342,8 +1478,17 @@
       <c r="K10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M10" t="s">
+        <v>186</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="O10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>106</v>
       </c>
@@ -1375,7 +1520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>107</v>
       </c>
@@ -1407,7 +1552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>108</v>
       </c>
@@ -1432,14 +1577,14 @@
       <c r="I13" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="14" t="s">
         <v>9</v>
       </c>
       <c r="K13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>109</v>
       </c>
@@ -1471,7 +1616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>110</v>
       </c>
@@ -1503,7 +1648,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>111</v>
       </c>
@@ -1656,7 +1801,7 @@
       <c r="I20" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="14" t="s">
         <v>16</v>
       </c>
       <c r="K20" t="s">
@@ -1848,7 +1993,7 @@
       <c r="I26" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="J26" s="14" t="s">
         <v>22</v>
       </c>
       <c r="K26" t="s">
@@ -3838,17 +3983,17 @@
     </row>
     <row r="106" spans="2:11" ht="19" x14ac:dyDescent="0.25">
       <c r="B106" s="12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B107" s="13" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B107" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>